<commit_message>
add full entities from json
</commit_message>
<xml_diff>
--- a/rd_connect_entity_info.xlsx
+++ b/rd_connect_entity_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="154">
   <si>
     <t xml:space="preserve">entity</t>
   </si>
@@ -352,7 +352,70 @@
     <t xml:space="preserve">Requirement_to_sign_a_material_transfer_agreement</t>
   </si>
   <si>
-    <t xml:space="preserve">…</t>
+    <t xml:space="preserve">Does_the_informed_consent_include_the_option_for_patients_to_withdraw_sample_at_any_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available_Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient_s_data_linked_to_other_resources_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost_recovery_system_in_place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethical_Committee_approval_for_biobanking_activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select9246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please_specify_if_you_have_some_limitations_regarding_your_local_regulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are_the_biological_samples_collected_with_an_informed_consent_from_the_patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is_international_exchange_of_samples_considered_in_the_informed_consent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restriction_for_use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How_many_samples_are_distributed_per_year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If_no__please_specify_the_presumed_date_for_obtaining_the_approval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal_Data_Collected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do_you_have_a_sample_request_management_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is_an_ethics_board_decision_already_available_for_the_use_of_the_samples_in_research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type_of_consent_is_obtained_from_the_patients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please_specify_restriction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific_procedure_for_access_to_raw_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dedicated_policy_for_return_of_results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If_yes__please_specify_the_starting_date_of_the_approval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other4838</t>
   </si>
   <si>
     <t xml:space="preserve">bb_contribution</t>
@@ -361,13 +424,64 @@
     <t xml:space="preserve">Is_your_entire_sample_collection_available_for_the_RD-Connect_Catalogue</t>
   </si>
   <si>
+    <t xml:space="preserve">If_not__please_specify_what_type_of_collections_can_be_publicly_available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other_remarks_or_questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You_agree_to_distribute_samples_to_investigators_involved_in_rare_disease_research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please_write_a_few_lines_explaining_why_you_would_like_your_biobank_to_join_RD-Connect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You_are_willing_to_accept_the_terms_of_the_RD-Connect_general_charter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select8778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You_agree_to_publish_your_available_collections_on_the_RD-Connect_platform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your_biobank_will_retain_ownership__control_and_legal_liability_of_the_biological_samples__RD-Connect_does_not_take_responsibility_for_the_handling_to_the_samples_</t>
+  </si>
+  <si>
     <t xml:space="preserve">reg_accessibility</t>
   </si>
   <si>
-    <t xml:space="preserve">infromation provided in rdconeect id card- Accessibility</t>
+    <t xml:space="preserve">Has_the_registry_a_Data_Access_Committee_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If_yes__please_provide_the_Data_Access_Committee_webpage</t>
   </si>
   <si>
     <t xml:space="preserve">Data_Access_Agreement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do_you_use_a_Data_Access_Agreement_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scientific publications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abstract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document__if_available_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journal</t>
   </si>
 </sst>
 </file>
@@ -448,7 +562,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -459,6 +573,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -538,17 +656,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:J166"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C104" activeCellId="0" sqref="C104"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A75" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A99" activeCellId="0" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="96.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1341,51 +1459,291 @@
         <v>71</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B99" s="0" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B102" s="0" t="s">
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B104" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="C104" s="0" t="s">
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="0" t="s">
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="0" t="s">
-        <v>110</v>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B131" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B132" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B133" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B134" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B135" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B136" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B137" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B138" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B139" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B143" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B144" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B145" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B146" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B147" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B148" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B149" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B150" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B151" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B152" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B153" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B154" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B161" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B162" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B163" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B164" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B165" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B166" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
load lists and dicts to emx
</commit_message>
<xml_diff>
--- a/rd_connect_entity_info.xlsx
+++ b/rd_connect_entity_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="165">
   <si>
     <t xml:space="preserve">entity</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">ID</t>
   </si>
   <si>
+    <t xml:space="preserve">OrganizationID</t>
+  </si>
+  <si>
     <t xml:space="preserve">diseases</t>
   </si>
   <si>
@@ -106,9 +109,6 @@
     <t xml:space="preserve">timestamp</t>
   </si>
   <si>
-    <t xml:space="preserve">OrganizationID</t>
-  </si>
-  <si>
     <t xml:space="preserve">Organisation ID/ (biobank ID)</t>
   </si>
   <si>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">Standardized_case-inclusion_and-exclusion_criteria</t>
   </si>
   <si>
-    <t xml:space="preserve">_fieldsDispla</t>
+    <t xml:space="preserve">_fieldsDisplay</t>
   </si>
   <si>
     <t xml:space="preserve">core</t>
@@ -232,10 +232,7 @@
     <t xml:space="preserve">Additional_networks_inventories</t>
   </si>
   <si>
-    <t xml:space="preserve">_fieldsDisplay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact</t>
+    <t xml:space="preserve">contacts</t>
   </si>
   <si>
     <t xml:space="preserve">last name</t>
@@ -247,6 +244,9 @@
     <t xml:space="preserve">email</t>
   </si>
   <si>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
     <t xml:space="preserve">main</t>
   </si>
   <si>
@@ -460,7 +460,7 @@
     <t xml:space="preserve">Do_you_use_a_Data_Access_Agreement_</t>
   </si>
   <si>
-    <t xml:space="preserve">scientific publications</t>
+    <t xml:space="preserve">Scientific publications</t>
   </si>
   <si>
     <t xml:space="preserve">Year</t>
@@ -479,6 +479,42 @@
   </si>
   <si>
     <t xml:space="preserve">Journal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bb_core</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional_Biomaterial_available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional_Origin_of_collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How_many_RD_are_in_the_registry_biobank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use_of_collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Origin_of_collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional_Biomaterial_prepared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomaterial_Available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage_of_rare_diseases_in_your_registry_biobank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomaterial_prepared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional_Use_of_collection</t>
   </si>
 </sst>
 </file>
@@ -488,7 +524,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -509,11 +545,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -564,7 +595,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -579,10 +610,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -662,10 +689,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J154"/>
+  <dimension ref="A1:J198"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A86" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B121" activeCellId="0" sqref="B121"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B62" activeCellId="0" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -755,142 +782,135 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>15</v>
-      </c>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="0" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="C18" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>33</v>
@@ -898,35 +918,41 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C24" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D24" s="0" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -934,37 +960,34 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -974,54 +997,40 @@
         <v>38</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>48</v>
-      </c>
+      <c r="B32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -1031,11 +1040,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>11</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1045,16 +1056,10 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -1065,10 +1070,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -1082,39 +1087,69 @@
         <v>49</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>54</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>49</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>55</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>49</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>56</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>49</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>57</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>49</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1122,7 +1157,7 @@
         <v>49</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1130,7 +1165,7 @@
         <v>49</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1138,7 +1173,7 @@
         <v>49</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1146,7 +1181,7 @@
         <v>49</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1154,7 +1189,7 @@
         <v>49</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1162,7 +1197,7 @@
         <v>49</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,7 +1205,7 @@
         <v>49</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1178,7 +1213,7 @@
         <v>49</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,7 +1221,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1194,7 +1229,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,7 +1237,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1210,123 +1245,123 @@
         <v>49</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>77</v>
+        <v>70</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="B58" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>41</v>
+        <v>71</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="B63" s="0" t="s">
-        <v>44</v>
+        <v>70</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="0" t="s">
-        <v>47</v>
+      <c r="B64" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B65" s="0" t="s">
-        <v>81</v>
+      <c r="B65" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1334,7 +1369,7 @@
         <v>78</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1342,7 +1377,7 @@
         <v>78</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,7 +1385,7 @@
         <v>78</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1358,7 +1393,7 @@
         <v>78</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1366,7 +1401,7 @@
         <v>78</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1374,7 +1409,7 @@
         <v>78</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1382,7 +1417,7 @@
         <v>78</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1390,7 +1425,7 @@
         <v>78</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,7 +1433,7 @@
         <v>78</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,63 +1441,63 @@
         <v>78</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1470,7 +1505,7 @@
         <v>88</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1478,7 +1513,7 @@
         <v>88</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>96</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1486,7 +1521,7 @@
         <v>88</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1494,7 +1529,7 @@
         <v>88</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1502,7 +1537,7 @@
         <v>88</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1510,7 +1545,7 @@
         <v>88</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,7 +1553,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1526,7 +1561,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1534,7 +1569,7 @@
         <v>88</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,7 +1577,7 @@
         <v>88</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1550,7 +1585,7 @@
         <v>88</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1558,7 +1593,7 @@
         <v>88</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1566,95 +1601,95 @@
         <v>88</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>109</v>
+        <v>88</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>110</v>
+        <v>88</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>111</v>
+        <v>88</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>112</v>
+        <v>88</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>113</v>
+        <v>88</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>114</v>
+        <v>88</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B104" s="3" t="s">
-        <v>115</v>
+      <c r="B104" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B105" s="3" t="s">
-        <v>116</v>
+      <c r="B105" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B106" s="3" t="s">
-        <v>117</v>
+      <c r="B106" s="0" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1662,7 +1697,7 @@
         <v>107</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1670,7 +1705,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,7 +1713,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,7 +1721,7 @@
         <v>107</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,7 +1729,7 @@
         <v>107</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1702,7 +1737,7 @@
         <v>107</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1710,7 +1745,7 @@
         <v>107</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1718,7 +1753,7 @@
         <v>107</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1726,7 +1761,7 @@
         <v>107</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,7 +1769,7 @@
         <v>107</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,7 +1777,7 @@
         <v>107</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,7 +1785,7 @@
         <v>107</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1758,7 +1793,7 @@
         <v>107</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1766,175 +1801,175 @@
         <v>107</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="4" t="s">
-        <v>131</v>
+      <c r="A121" s="0" t="s">
+        <v>107</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>11</v>
+        <v>123</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B129" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
+      <c r="B130" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B130" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
-        <v>131</v>
-      </c>
       <c r="B131" s="3" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1942,7 +1977,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>145</v>
+        <v>12</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1950,7 +1985,7 @@
         <v>141</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>125</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1958,7 +1993,7 @@
         <v>141</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1966,7 +2001,7 @@
         <v>141</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,71 +2009,423 @@
         <v>141</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>70</v>
+        <v>142</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="B154" s="3" t="s">
-        <v>70</v>
+      <c r="B158" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B167" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B168" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B171" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>